<commit_message>
update code and figure and tables used in manuscript
</commit_message>
<xml_diff>
--- a/parameters/Task22_Param_Ranges_AFIR_Tfold.xlsx
+++ b/parameters/Task22_Param_Ranges_AFIR_Tfold.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steinanf/git/TMDD_EndogenousLigand/parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D09FFE-46DA-984B-8102-80FA30AFBD52}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CA3C30-436F-B346-94A4-6EA9AB1E696F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="480" windowWidth="26440" windowHeight="16720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="580" yWindow="460" windowWidth="26440" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Task05_Param_Summary" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1349,8 +1351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="163" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="163" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>